<commit_message>
SOECENT-147 | update cloudinary script and add timeline data (#35)
* SOECENT-147 | update cloudinary script

* convert timeline data; update timeline

* fixup xlsx to json conversion for year

* update timeline lineart

* add spacing to full width timeline details

* SOECENT-147 | add alternative body display (#36)

* test

* remove delay

* fixup sizing

* remove photo dupe

* remove console.log

* fixup dupe image

* update semantic html structure for timeline list

* update timeline data
</commit_message>
<xml_diff>
--- a/scripts/files/cloudinary_images.xlsx
+++ b/scripts/files/cloudinary_images.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B161"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,311 +412,1287 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Squiggle_01_iezjdh</v>
+        <v>Barbara_Liskov_computer_scientist_2010_bzar2y</v>
       </c>
       <c r="B2" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739489566/Squiggle_01_iezjdh.svg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265430/Barbara_Liskov_computer_scientist_2010_bzar2y.jpg</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>williamHewlett_yezmww</v>
+        <v>3523ScheinmanHydrArm_i9xqlr</v>
       </c>
       <c r="B3" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481953/williamHewlett_yezmww.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265429/3523ScheinmanHydrArm_i9xqlr.jpg</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>irmgardFluggeLotz_silhouette_gfjjgm</v>
+        <v>tarpeh_rod_searcy_hml0tu</v>
       </c>
       <c r="B4" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481951/irmgardFluggeLotz_silhouette_gfjjgm.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265428/tarpeh_rod_searcy_hml0tu.jpg</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Ryan-High-Voltage-Laboratory_rinsml</v>
+        <v>bb752wg6044_ajr0ww</v>
       </c>
       <c r="B5" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481950/Ryan-High-Voltage-Laboratory_rinsml.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265427/bb752wg6044_ajr0ww.jpg</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>maeJemison_crwmks</v>
+        <v>Francis_and_Brad-Press_Day_mgtwwl</v>
       </c>
       <c r="B6" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481947/maeJemison_crwmks.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265426/Francis_and_Brad-Press_Day_mgtwwl.jpg</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>machineSilhouette_xnmpup</v>
+        <v>james_gibbons_1984_d9vof3</v>
       </c>
       <c r="B7" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481947/machineSilhouette_xnmpup.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265425/james_gibbons_1984_d9vof3.jpg</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>packardBell_rgwp2j</v>
+        <v>1024px-Admiral_Bobby_Ray_Inman__official_CIA_photo__1983_sha4yp</v>
       </c>
       <c r="B8" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481946/packardBell_rgwp2j.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265424/1024px-Admiral_Bobby_Ray_Inman__official_CIA_photo__1983_sha4yp.jpg</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>130704-9205_silhouette_j9uj3j</v>
+        <v>mae_jamison_commencement_bvmth7</v>
       </c>
       <c r="B9" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481946/130704-9205_silhouette_j9uj3j.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265424/mae_jamison_commencement_bvmth7.jpg</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>robotFlipped_e0kkk6</v>
+        <v>william_durand_lwurlu</v>
       </c>
       <c r="B10" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481945/robotFlipped_e0kkk6.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265423/william_durand_lwurlu.jpg</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>group_silhouette_wmmyl3</v>
+        <v>SC0122_1998-144_b02_Computers_1985_0030_ma4z7u</v>
       </c>
       <c r="B11" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1739481944/group_silhouette_wmmyl3.png</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265422/SC0122_1998-144_b02_Computers_1985_0030_ma4z7u.jpg</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>william-w-hansen_osvbzp</v>
+        <v>ocean_one_fwy7nd</v>
       </c>
       <c r="B12" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861407/william-w-hansen_osvbzp.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265421/ocean_one_fwy7nd.jpg</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>prof-edward-2_xecpct</v>
+        <v>jennifer-widom_srdoc9</v>
       </c>
       <c r="B13" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861406/prof-edward-2_xecpct.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265420/jennifer-widom_srdoc9.jpg</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>mark-2-2_jf2xmm</v>
+        <v>hanrahan_pat_1_mxp4yf</v>
       </c>
       <c r="B14" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861407/mark-2-2_jf2xmm.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265419/hanrahan_pat_1_mxp4yf.jpg</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>felix-bloch_dg6ato</v>
+        <v>philip-wong-profile_EWS_h3zpoo</v>
       </c>
       <c r="B15" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861406/felix-bloch_dg6ato.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265418/philip-wong-profile_EWS_h3zpoo.jpg</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>redevelopment_vprsob</v>
+        <v>murray_and_taber_ibiiju</v>
       </c>
       <c r="B16" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861405/redevelopment_vprsob.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265417/murray_and_taber_ibiiju.jpg</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>stephen-p-timoshenko_rr0uke</v>
+        <v>oussama_khatib_dpohpx</v>
       </c>
       <c r="B17" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861405/stephen-p-timoshenko_rr0uke.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265416/oussama_khatib_dpohpx.jpg</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>david-packard-william_l1tf3k</v>
+        <v>jeffrey_ullman_azhmrn</v>
       </c>
       <c r="B18" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861405/david-packard-william_l1tf3k.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265415/jeffrey_ullman_azhmrn.jpg</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>new-spaces-and-expanding-influence_dcvv7j</v>
+        <v>google_gathering_2005_lvouaq</v>
       </c>
       <c r="B19" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861405/new-spaces-and-expanding-influence_dcvv7j.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265414/google_gathering_2005_lvouaq.jpg</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>prof-edward-1_cfwklw</v>
+        <v>harris_j_ryan_wmnw5e</v>
       </c>
       <c r="B20" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861405/prof-edward-1_cfwklw.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265414/harris_j_ryan_wmnw5e.jpg</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>bridging-worlds_ma3ixq</v>
+        <v>hewlett-packard_dedication_rm7du9</v>
       </c>
       <c r="B21" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861404/bridging-worlds_ma3ixq.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265413/hewlett-packard_dedication_rm7du9.jpg</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>mark-2_nncexe</v>
+        <v>pk304kr0557_EWS_k7kxcv</v>
       </c>
       <c r="B22" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738861404/mark-2_nncexe.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265412/pk304kr0557_EWS_k7kxcv.jpg</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>stangord-campus-1948_d7gus7</v>
+        <v>linear_accelerator_first_section_pdzh0j</v>
       </c>
       <c r="B23" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738812005/stangord-campus-1948_d7gus7.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265411/linear_accelerator_first_section_pdzh0j.jpg</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>BookCover_optimized_piu8wz</v>
+        <v>Jelena_Vuckovic_High-Res_tigsje</v>
       </c>
       <c r="B24" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1738811648/BookCover_optimized_piu8wz.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265410/Jelena_Vuckovic_High-Res_tigsje.jpg</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>mae-johnson-nasa_mdcnkj</v>
+        <v>SC0122_1992-003_b303_X269-007_twv1p4</v>
       </c>
       <c r="B25" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737062695/mae-johnson-nasa_mdcnkj.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265409/SC0122_1992-003_b303_X269-007_twv1p4.jpg</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>stanford-dish_cgacpq</v>
+        <v>AlexandraBoehm_01_Hi-Res_9828_ro1a88</v>
       </c>
       <c r="B26" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737062695/stanford-dish_cgacpq.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265408/AlexandraBoehm_01_Hi-Res_9828_ro1a88.jpg</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>first-remote-class_kpaahw</v>
+        <v>linvill_daughter_candance_qic2j4</v>
       </c>
       <c r="B27" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737062695/first-remote-class_kpaahw.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265407/linvill_daughter_candance_qic2j4.jpg</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>1936-1944_-_Stanford_Engineering_s_second_Dean_s8t8aa</v>
+        <v>Owen_Garriott_NASA_pufv2m</v>
       </c>
       <c r="B28" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060928/1936-1944_-_Stanford_Engineering_s_second_Dean_s8t8aa.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265406/Owen_Garriott_NASA_pufv2m.jpg</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>1944_-_Army_Specialized_Training_Program_1_tsurqu</v>
+        <v>martin_hellman_1978_n6m3s5</v>
       </c>
       <c r="B29" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060927/1944_-_Army_Specialized_Training_Program_1_tsurqu.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265405/martin_hellman_1978_n6m3s5.jpg</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>skilling_umi5ca</v>
+        <v>hewlett_center_exterior_aeutsi</v>
       </c>
       <c r="B30" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060928/skilling_umi5ca.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265404/hewlett_center_exterior_aeutsi.jpg</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>1943_-_Training_for_war_qld0yb</v>
+        <v>U7477_mvmcyh</v>
       </c>
       <c r="B31" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060928/1943_-_Training_for_war_qld0yb.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265403/U7477_mvmcyh.jpg</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>1939_-_Inventors_of_the_klystron_aipcnt</v>
+        <v>dschoolcohort_brgwch</v>
       </c>
       <c r="B32" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060928/1939_-_Inventors_of_the_klystron_aipcnt.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265402/dschoolcohort_brgwch.jpg</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>terman_uv6swj</v>
+        <v>codeinplace_td2zef</v>
       </c>
       <c r="B33" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060928/terman_uv6swj.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265402/codeinplace_td2zef.jpg</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>1926_-_The_largest_university_electrical_lab_of_its_time_xdomjd</v>
+        <v>Stanford_HAI_1381-_web_ylpw8q</v>
       </c>
       <c r="B34" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060927/1926_-_The_largest_university_electrical_lab_of_its_time_xdomjd.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265401/Stanford_HAI_1381-_web_ylpw8q.jpg</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>1944_-_Stanford_Engineering_s_third_Dean_leujr9</v>
+        <v>rm634fy8400_m1dxsp</v>
       </c>
       <c r="B35" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060927/1944_-_Stanford_Engineering_s_third_Dean_leujr9.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265400/rm634fy8400_m1dxsp.jpg</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>1910-1915_-_The_Engineering_Corner_lafzrp</v>
+        <v>3523ScheinmanHydrArm_oxkyl8</v>
       </c>
       <c r="B36" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060927/1910-1915_-_The_Engineering_Corner_lafzrp.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265234/3523ScheinmanHydrArm_oxkyl8.jpg</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>1939_-_Aviation_and_aeronautical_engineering_bwguek</v>
+        <v>WelcomeDay_GroupPhotos_9.26.24_01_O5A0256_ghau9a</v>
       </c>
       <c r="B37" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060927/1939_-_Aviation_and_aeronautical_engineering_bwguek.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265232/WelcomeDay_GroupPhotos_9.26.24_01_O5A0256_ghau9a.jpg</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>1937_-_Foundational_technology_in_the_burgeoning_microwave_industry_tvqbqy</v>
+        <v>hewlett_packard_hoarz7</v>
       </c>
       <c r="B38" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060927/1937_-_Foundational_technology_in_the_burgeoning_microwave_industry_tvqbqy.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265231/hewlett_packard_hoarz7.jpg</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>1939_-_Model_200A_precision_audio_oscillator_qlyawb</v>
+        <v>nuclear_reactor_xgxrqi</v>
       </c>
       <c r="B39" t="str">
-        <v>https://res.cloudinary.com/dsqi5touf/image/upload/v1737060927/1939_-_Model_200A_precision_audio_oscillator_qlyawb.jpg</v>
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265231/nuclear_reactor_xgxrqi.jpg</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Majumdar_oyx924</v>
+      </c>
+      <c r="B40" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265230/Majumdar_oyx924.jpg</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>IA_35_EllenOchoa_NASAviaFlickr_29320023973_856ebf4a77_o-1_qftsts</v>
+      </c>
+      <c r="B41" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265229/IA_35_EllenOchoa_NASAviaFlickr_29320023973_856ebf4a77_o-1_qftsts.webp</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>james_plummer_n9oena</v>
+      </c>
+      <c r="B42" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265227/james_plummer_n9oena.jpg</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>kenneth_arrow_wexcgd</v>
+      </c>
+      <c r="B43" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265227/kenneth_arrow_wexcgd.jpg</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>xm262js0452_pu6tmf</v>
+      </c>
+      <c r="B44" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265226/xm262js0452_pu6tmf.jpg</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>fn928pv3867_voo2ky</v>
+      </c>
+      <c r="B45" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265225/fn928pv3867_voo2ky.jpg</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>high_voltage_laboratory_moonff</v>
+      </c>
+      <c r="B46" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265224/high_voltage_laboratory_moonff.jpg</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>john_hennessy_giilx7</v>
+      </c>
+      <c r="B47" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265223/john_hennessy_giilx7.jpg</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>david-kelley_ztssoh</v>
+      </c>
+      <c r="B48" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265223/david-kelley_ztssoh.jpg</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>SA_inst_team-031804-1712w_b1i418</v>
+      </c>
+      <c r="B49" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265221/SA_inst_team-031804-1712w_b1i418.jpg</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>vr758kf1949_nv217v</v>
+      </c>
+      <c r="B50" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265221/vr758kf1949_nv217v.jpg</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>computation_corner_dedication_j3dzmf</v>
+      </c>
+      <c r="B51" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265219/computation_corner_dedication_j3dzmf.jpg</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>ronald_bracewell_1959_dtua2a</v>
+      </c>
+      <c r="B52" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265219/ronald_bracewell_1959_dtua2a.jpg</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>SC0122_1981-087_b01_f005_jzcowg</v>
+      </c>
+      <c r="B53" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265217/SC0122_1981-087_b01_f005_jzcowg.jpg</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>multivators_qdggyv</v>
+      </c>
+      <c r="B54" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265216/multivators_qdggyv.jpg</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>DF-SC-97-01109_zpm0cf</v>
+      </c>
+      <c r="B55" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265215/DF-SC-97-01109_zpm0cf.jpg</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>vinton_cerf_ofhvxu</v>
+      </c>
+      <c r="B56" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265215/vinton_cerf_ofhvxu.jpg</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>00007001_0001.jpg_electrical_engineers_up1grc</v>
+      </c>
+      <c r="B57" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265213/00007001_0001.jpg_electrical_engineers_up1grc.jpg</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>kn908nr7305_dxr5db</v>
+      </c>
+      <c r="B58" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265213/kn908nr7305_dxr5db.jpg</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Poon_microstimulator_w_penny_j5psr3</v>
+      </c>
+      <c r="B59" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265212/Poon_microstimulator_w_penny_j5psr3.jpg</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>00008355_001_izvi7r</v>
+      </c>
+      <c r="B60" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265211/00008355_001_izvi7r.jpg</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>STS047-37-003_large_rk5g83</v>
+      </c>
+      <c r="B61" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265210/STS047-37-003_large_rk5g83.jpg</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>visitors_from_france_e7pbw3</v>
+      </c>
+      <c r="B62" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265209/visitors_from_france_e7pbw3.jpg</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>SC1041_SAIL_CartDeck_2_gao7tp</v>
+      </c>
+      <c r="B63" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265208/SC1041_SAIL_CartDeck_2_gao7tp.jpg</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>00005705_0023_hf0ufd</v>
+      </c>
+      <c r="B64" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265207/00005705_0023_hf0ufd.jpg</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>00021082_004_ptdepc</v>
+      </c>
+      <c r="B65" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265206/00021082_004_ptdepc.jpg</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>zm384pb3271_t5ac1m</v>
+      </c>
+      <c r="B66" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265205/zm384pb3271_t5ac1m.jpg</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Shenoy_MG_6677_jqo0uy</v>
+      </c>
+      <c r="B67" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265205/Shenoy_MG_6677_jqo0uy.jpg</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>00018323_004_myytao</v>
+      </c>
+      <c r="B68" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265204/00018323_004_myytao.jpg</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>mb981vc1736_qaa7ma</v>
+      </c>
+      <c r="B69" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265202/mb981vc1736_qaa7ma.jpg</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>PC0062_2008-194_SEQ_04_015_ziycgm</v>
+      </c>
+      <c r="B70" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265201/PC0062_2008-194_SEQ_04_015_ziycgm.jpg</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Jennifer_Widom_preferred__High-Res_mbyvny</v>
+      </c>
+      <c r="B71" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265201/Jennifer_Widom_preferred__High-Res_mbyvny.jpg</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>00006962_0001_opgfxn</v>
+      </c>
+      <c r="B72" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265199/00006962_0001_opgfxn.jpg</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>faculty_meeting_1972_cyq3gl</v>
+      </c>
+      <c r="B73" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265198/faculty_meeting_1972_cyq3gl.jpg</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Deisseroth_SteveFisch_zhdfl2</v>
+      </c>
+      <c r="B74" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265197/Deisseroth_SteveFisch_zhdfl2.jpg</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>fs075wb6787_i8hbd2</v>
+      </c>
+      <c r="B75" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265197/fs075wb6787_i8hbd2.jpg</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Copy_of_00014490_015_mfcej3</v>
+      </c>
+      <c r="B76" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265196/Copy_of_00014490_015_mfcej3.jpg</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>br440jc7470_lhb21j</v>
+      </c>
+      <c r="B77" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265195/br440jc7470_lhb21j.jpg</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>terman_qm422bp1949_5.57.39_PM_pkfzoq</v>
+      </c>
+      <c r="B78" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265195/terman_qm422bp1949_5.57.39_PM_pkfzoq.jpg</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Copy_of_00007204_0003.jpg_Guggehneim_Lab_yvaovr</v>
+      </c>
+      <c r="B79" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265194/Copy_of_00007204_0003.jpg_Guggehneim_Lab_yvaovr.jpg</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>sebastian-thrun_ybkibn</v>
+      </c>
+      <c r="B80" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265193/sebastian-thrun_ybkibn.jpg</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>2023_08_11_110846_cezues</v>
+      </c>
+      <c r="B81" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265192/2023_08_11_110846_cezues.jpg</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>00015013_0001_cw3g42</v>
+      </c>
+      <c r="B82" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265192/00015013_0001_cw3g42.jpg</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>PC0139_Persis_Drell_2014-09-05_2866_dsvp3h</v>
+      </c>
+      <c r="B83" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265191/PC0139_Persis_Drell_2014-09-05_2866_dsvp3h.jpg</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>fz107qj0976_elakil</v>
+      </c>
+      <c r="B84" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265190/fz107qj0976_elakil.jpg</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Copy_of_00012017_005_e0a3bb</v>
+      </c>
+      <c r="B85" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265190/Copy_of_00012017_005_e0a3bb.jpg</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Copy_of_00007002_0011.jpg_engineering_lab_exterior_tkaady</v>
+      </c>
+      <c r="B86" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265189/Copy_of_00007002_0011.jpg_engineering_lab_exterior_tkaady.jpg</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>wx455zm5299_ntjq2o</v>
+      </c>
+      <c r="B87" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265189/wx455zm5299_ntjq2o.jpg</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Fig.1d_qkhzka</v>
+      </c>
+      <c r="B88" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265188/Fig.1d_qkhzka.jpg</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>jx362js8604_blagdq</v>
+      </c>
+      <c r="B89" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265187/jx362js8604_blagdq.jpg</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>00006854_0002_rp3ytt</v>
+      </c>
+      <c r="B90" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265187/00006854_0002_rp3ytt.jpg</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>00018325_004_s9kcul</v>
+      </c>
+      <c r="B91" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265186/00018325_004_s9kcul.jpg</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>xx798bb1141_zbiqrv</v>
+      </c>
+      <c r="B92" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265185/xx798bb1141_zbiqrv.jpg</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>00007004_0001_rdznf1</v>
+      </c>
+      <c r="B93" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265185/00007004_0001_rdznf1.jpg</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>00020166_001_uko5kx</v>
+      </c>
+      <c r="B94" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265184/00020166_001_uko5kx.jpg</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>hugh_skilling_uzvnx3</v>
+      </c>
+      <c r="B95" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265183/hugh_skilling_uzvnx3.jpg</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>00006955_0005_quv7kg</v>
+      </c>
+      <c r="B96" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265183/00006955_0005_quv7kg.jpg</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>stanley-2005_zwcpcx</v>
+      </c>
+      <c r="B97" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265182/stanley-2005_zwcpcx.jpg</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>00002098_0003_tng0js</v>
+      </c>
+      <c r="B98" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265182/00002098_0003_tng0js.jpg</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>Map_1966_nmlwwh</v>
+      </c>
+      <c r="B99" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265181/Map_1966_nmlwwh.jpg</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>00007005_0006_q8nhmq</v>
+      </c>
+      <c r="B100" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265180/00007005_0006_q8nhmq.jpg</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>00005967_0003_krk8lw</v>
+      </c>
+      <c r="B101" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265179/00005967_0003_krk8lw.jpg</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>fred_terman_1977_k6fsc1</v>
+      </c>
+      <c r="B102" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265179/fred_terman_1977_k6fsc1.jpg</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>SC0122_s1_b268_f06_1546-11_rb5f1b</v>
+      </c>
+      <c r="B103" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265178/SC0122_s1_b268_f06_1546-11_rb5f1b.jpg</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>russ_altman_gk8axg</v>
+      </c>
+      <c r="B104" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265178/russ_altman_gk8axg.jpg</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>PC0062_2008-194_AERIALS_01_009_wsktco</v>
+      </c>
+      <c r="B105" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265177/PC0062_2008-194_AERIALS_01_009_wsktco.jpg</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>john_g_herriot_fwbols</v>
+      </c>
+      <c r="B106" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265176/john_g_herriot_fwbols.jpg</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>railroad_car_geoxb2</v>
+      </c>
+      <c r="B107" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265176/railroad_car_geoxb2.jpg</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>mechanical_engineering_student_t9m8ee</v>
+      </c>
+      <c r="B108" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265175/mechanical_engineering_student_t9m8ee.jpg</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>experimental_power_lines_lbvixo</v>
+      </c>
+      <c r="B109" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265174/experimental_power_lines_lbvixo.jpg</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>00002098_0011_ge5nki</v>
+      </c>
+      <c r="B110" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265174/00002098_0011_ge5nki.jpg</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>mechanical_engineering_student_b4maik</v>
+      </c>
+      <c r="B111" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265173/mechanical_engineering_student_b4maik.jpg</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>flugge-lotz_jieewa</v>
+      </c>
+      <c r="B112" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265172/flugge-lotz_jieewa.jpg</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>PC0141_b10_Engineering_Corner_0511_EWS2_yxv22y</v>
+      </c>
+      <c r="B113" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265172/PC0141_b10_Engineering_Corner_0511_EWS2_yxv22y.jpg</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>Hoover_EmergingTechEvent_11-14-23_PatrickBeaudouin_IMG_0478_s7ge4w</v>
+      </c>
+      <c r="B114" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265170/Hoover_EmergingTechEvent_11-14-23_PatrickBeaudouin_IMG_0478_s7ge4w.jpg</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>meindl_mitterand_jobs_u3vm9p</v>
+      </c>
+      <c r="B115" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265169/meindl_mitterand_jobs_u3vm9p.jpg</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>00002098_0012_dkks2x</v>
+      </c>
+      <c r="B116" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265168/00002098_0012_dkks2x.jpg</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>mark_iii_linear_accelerator_rcmzad</v>
+      </c>
+      <c r="B117" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265168/mark_iii_linear_accelerator_rcmzad.jpg</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>merkle_hellman_diffie_r007vv</v>
+      </c>
+      <c r="B118" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265167/merkle_hellman_diffie_r007vv.jpg</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>3d-bioprinting_zzau8e</v>
+      </c>
+      <c r="B119" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265167/3d-bioprinting_zzau8e.jpg</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>pettit_jn566pd7749_hgribe</v>
+      </c>
+      <c r="B120" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265166/pettit_jn566pd7749_hgribe.jpg</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>SC0122_s1_b271_f05_6030-09_c8jpbq</v>
+      </c>
+      <c r="B121" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265165/SC0122_s1_b271_f05_6030-09_c8jpbq.jpg</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>stanford_solar_car_hf0620</v>
+      </c>
+      <c r="B122" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265165/stanford_solar_car_hf0620.jpg</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>PC0141_b07_Timoshenko_0120_ou3zaf</v>
+      </c>
+      <c r="B123" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265164/PC0141_b07_Timoshenko_0120_ou3zaf.jpg</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>ginzton_kaplan_bggokw</v>
+      </c>
+      <c r="B124" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265164/ginzton_kaplan_bggokw.jpg</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>00002390_0001_ysrdsn</v>
+      </c>
+      <c r="B125" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265163/00002390_0001_ysrdsn.jpg</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>PC0141_b12_Engineering_Corner_0172_nxsc55</v>
+      </c>
+      <c r="B126" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265162/PC0141_b12_Engineering_Corner_0172_nxsc55.jpg</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>A-CAM-2022SE-138_bcjho9</v>
+      </c>
+      <c r="B127" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265162/A-CAM-2022SE-138_bcjho9.jpg</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>jh189cy1846_bzmmv6</v>
+      </c>
+      <c r="B128" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265162/jh189cy1846_bzmmv6.jpg</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>P8025899_w4032_q10_tamdi6</v>
+      </c>
+      <c r="B129" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265161/P8025899_w4032_q10_tamdi6.jpg</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>zx844pk9013_j3dof4</v>
+      </c>
+      <c r="B130" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265160/zx844pk9013_j3dof4.jpg</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>SC0122_s1_b278_f04_C388-13_pyqfce</v>
+      </c>
+      <c r="B131" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265159/SC0122_s1_b278_f04_C388-13_pyqfce.jpg</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>doerr_school_jdpsi0</v>
+      </c>
+      <c r="B132" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265158/doerr_school_jdpsi0.jpg</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>wd899qz9103_00_0001_EWS_vhj8r8</v>
+      </c>
+      <c r="B133" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265158/wd899qz9103_00_0001_EWS_vhj8r8.jpg</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>pars_pro_toto_orkqco</v>
+      </c>
+      <c r="B134" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265158/pars_pro_toto_orkqco.jpg</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>theodore_hoover_yiel9t</v>
+      </c>
+      <c r="B135" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265157/theodore_hoover_yiel9t.jpg</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>john_mccarthy_chess_pqxfgp</v>
+      </c>
+      <c r="B136" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265155/john_mccarthy_chess_pqxfgp.jpg</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>SC0122_s1_b278_f10_C958-007_lqdmba</v>
+      </c>
+      <c r="B137" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265156/SC0122_s1_b278_f10_C958-007_lqdmba.jpg</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>students_with_professor_shah_s8vayt</v>
+      </c>
+      <c r="B138" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265156/students_with_professor_shah_s8vayt.jpg</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>hansen_accelerator_ylgrdb</v>
+      </c>
+      <c r="B139" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265154/hansen_accelerator_ylgrdb.jpg</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>Map_1966_j9hpyj</v>
+      </c>
+      <c r="B140" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265154/Map_1966_j9hpyj.jpg</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>SC0122_s1_b278_f01_C076-02_qvsla2</v>
+      </c>
+      <c r="B141" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265152/SC0122_s1_b278_f01_C076-02_qvsla2.jpg</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>SUBB_SD_Aerial_Garden_Court_jsfs5l</v>
+      </c>
+      <c r="B142" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265152/SUBB_SD_Aerial_Garden_Court_jsfs5l.jpg</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>PC0062_s1_b06_f70_uqytkq</v>
+      </c>
+      <c r="B143" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265149/PC0062_s1_b06_f70_uqytkq.jpg</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>Hoover_EmergingTechEvent_QE_11-14-23_PatrickBeaudouin_PTB_2163_kt5faz</v>
+      </c>
+      <c r="B144" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265149/Hoover_EmergingTechEvent_QE_11-14-23_PatrickBeaudouin_PTB_2163_kt5faz.jpg</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>00007000_0009_rdq5ts</v>
+      </c>
+      <c r="B145" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265148/00007000_0009_rdq5ts.jpg</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>Cartoon_EWS_qtpizx</v>
+      </c>
+      <c r="B146" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265147/Cartoon_EWS_qtpizx.jpg</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>nz029jf0057_lmfjwr</v>
+      </c>
+      <c r="B147" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265146/nz029jf0057_lmfjwr.jpg</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>00019306_001_csiwis</v>
+      </c>
+      <c r="B148" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265145/00019306_001_csiwis.jpg</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>central-energy-facility-2015_nrngaz</v>
+      </c>
+      <c r="B149" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265144/central-energy-facility-2015_nrngaz.jpg</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>ck707sy2214_h2kuty</v>
+      </c>
+      <c r="B150" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265143/ck707sy2214_h2kuty.jpg</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>SC0122_s1_b269_f13_3354-11_qbh2ew</v>
+      </c>
+      <c r="B151" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265142/SC0122_s1_b269_f13_3354-11_qbh2ew.jpg</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>vq647dq9662_nc29rh</v>
+      </c>
+      <c r="B152" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265142/vq647dq9662_nc29rh.jpg</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>aerial-campus-view-2011_owdrjo</v>
+      </c>
+      <c r="B153" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265141/aerial-campus-view-2011_owdrjo.jpg</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>SC0122_s1_b267_f02_0115-01_uc3pdv</v>
+      </c>
+      <c r="B154" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265140/SC0122_s1_b267_f02_0115-01_uc3pdv.jpg</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>A-CAM-2022SE-178_bh3zwv</v>
+      </c>
+      <c r="B155" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265140/A-CAM-2022SE-178_bh3zwv.jpg</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>students_with_professor_shah_wajng8</v>
+      </c>
+      <c r="B156" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265139/students_with_professor_shah_wajng8.jpg</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>ginzton_accelerator_j1ee3v</v>
+      </c>
+      <c r="B157" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265139/ginzton_accelerator_j1ee3v.jpg</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>SC0122_s1_b269_f10_3000-09_np7kyh</v>
+      </c>
+      <c r="B158" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265138/SC0122_s1_b269_f10_3000-09_np7kyh.jpg</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>SC0122_s1_b278_f09_C832-06_wlr8rl</v>
+      </c>
+      <c r="B159" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265138/SC0122_s1_b278_f09_C832-06_wlr8rl.jpg</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>robot_demonstration_cpg8nr</v>
+      </c>
+      <c r="B160" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265137/robot_demonstration_cpg8nr.jpg</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>original_Google_server_lbqfqy</v>
+      </c>
+      <c r="B161" t="str">
+        <v>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265136/original_Google_server_lbqfqy.jpg</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B161"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>